<commit_message>
added stop wage assignment to ilao docassemble easy form list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2E5F3D-2352-4D28-8AF4-4F9FE388BC2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBAFD05-5215-4FF7-B7D5-31383CF13DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5295" windowWidth="29040" windowHeight="15840" xr2:uid="{D24EE308-1655-48F2-B0CD-E393F04C727C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/evict-tenant</t>
+  </si>
+  <si>
+    <t>Stop wage assignment</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/stop-wage-assignment-letter</t>
   </si>
 </sst>
 </file>
@@ -451,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8E61E4-2B81-4F91-90CA-45EAC44EC22D}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +539,14 @@
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -547,6 +561,7 @@
     <hyperlink ref="B5" r:id="rId5" xr:uid="{708B340C-0F53-470B-BB81-AD31C71A1614}"/>
     <hyperlink ref="B9" r:id="rId6" xr:uid="{C351A1B3-1071-4D4C-80EA-C02B556ED27D}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{59FF8705-B03A-411C-BF4C-5BC8D06EC1A0}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{B8411B4D-3208-4E8D-9BA2-4026E41AF3E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated feedback easy form list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\local-DA-easyforms-dev\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBAFD05-5215-4FF7-B7D5-31383CF13DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7EED65-6B4A-4E5D-A43E-333CCABCD438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5295" windowWidth="29040" windowHeight="15840" xr2:uid="{D24EE308-1655-48F2-B0CD-E393F04C727C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/stop-wage-assignment-letter</t>
+  </si>
+  <si>
+    <t>Request time off work due to domestic violence</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/request-time-work-due-domestic-abuse-letter</t>
   </si>
 </sst>
 </file>
@@ -457,15 +463,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8E61E4-2B81-4F91-90CA-45EAC44EC22D}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="104.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -535,23 +541,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B9">
-    <sortCondition ref="A2:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
+    <sortCondition ref="A2:A10"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{0BA79808-2665-45DC-A08F-ADBA3DB32B90}"/>
@@ -559,9 +573,10 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{1F04580F-DA75-4273-9192-B54929658F62}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{74BF8156-0B0B-49F2-BCB2-8D5A5C36DDFF}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{708B340C-0F53-470B-BB81-AD31C71A1614}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{C351A1B3-1071-4D4C-80EA-C02B556ED27D}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{C351A1B3-1071-4D4C-80EA-C02B556ED27D}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{59FF8705-B03A-411C-BF4C-5BC8D06EC1A0}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{B8411B4D-3208-4E8D-9BA2-4026E41AF3E6}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{B8411B4D-3208-4E8D-9BA2-4026E41AF3E6}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{39E534FA-B89C-4951-8041-044769B79749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added e-filing exemptions to easy form spreadsheet
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -5,37 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B084A5A-7DD3-4512-A7F1-ED7C746A1BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2733774-A1D7-4D23-99D5-49C380874F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5295" windowWidth="29040" windowHeight="15840" xr2:uid="{D24EE308-1655-48F2-B0CD-E393F04C727C}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -107,6 +97,24 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/appearance-e-filing</t>
+  </si>
+  <si>
+    <t>E-filing exemption - Appellate Court</t>
+  </si>
+  <si>
+    <t>E-filing exemption - Supreme Court</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/e-filing-exemption-circuit-court</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/e-filing-exemption-appellate-court</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/e-filing-exemption-supreme-court</t>
+  </si>
+  <si>
+    <t>E-filing exemption - Circuit Court</t>
   </si>
 </sst>
 </file>
@@ -468,20 +476,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8E61E4-2B81-4F91-90CA-45EAC44EC22D}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -497,7 +505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -505,7 +513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -513,7 +521,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -521,59 +529,83 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -582,15 +614,18 @@
     <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{0BA79808-2665-45DC-A08F-ADBA3DB32B90}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{CD1F53FD-5014-4ECB-B249-CD1C419AA221}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{1F04580F-DA75-4273-9192-B54929658F62}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{74BF8156-0B0B-49F2-BCB2-8D5A5C36DDFF}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{708B340C-0F53-470B-BB81-AD31C71A1614}"/>
-    <hyperlink ref="B11" r:id="rId6" xr:uid="{C351A1B3-1071-4D4C-80EA-C02B556ED27D}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{59FF8705-B03A-411C-BF4C-5BC8D06EC1A0}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{B8411B4D-3208-4E8D-9BA2-4026E41AF3E6}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{39E534FA-B89C-4951-8041-044769B79749}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Living Will program to easy forms spreadsheet
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmcnaughton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2733774-A1D7-4D23-99D5-49C380874F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -99,6 +108,9 @@
     <t>https://www.illinoislegalaid.org/legal-information/appearance-e-filing</t>
   </si>
   <si>
+    <t>E-filing exemption</t>
+  </si>
+  <si>
     <t>E-filing exemption - Appellate Court</t>
   </si>
   <si>
@@ -114,13 +126,16 @@
     <t>https://www.illinoislegalaid.org/legal-information/e-filing-exemption-supreme-court</t>
   </si>
   <si>
-    <t>E-filing exemption - Circuit Court</t>
+    <t>Living will</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/living-will</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,20 +491,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.44140625" customWidth="1"/>
+    <col min="1" max="1" width="44.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -505,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -513,7 +528,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -521,7 +536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -529,31 +544,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -561,7 +576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -569,7 +584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -577,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -585,47 +600,55 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
+  <sortState ref="A2:B11">
     <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B16" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B6" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="B8" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added respond to a lawsuit to easy form list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmcnaughton\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3143BEF-31D9-44F0-96D1-B882049AF414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -130,12 +121,18 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/living-will</t>
+  </si>
+  <si>
+    <t>Respond to a lawsuit</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/respond-lawsuit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -491,20 +488,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.453125" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -520,7 +517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -528,7 +525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -536,7 +533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -544,7 +541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -552,7 +549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -560,7 +557,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -568,7 +565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -576,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -584,7 +581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -592,7 +589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -600,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -608,7 +605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -616,39 +613,48 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
     <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B15" r:id="rId6"/>
-    <hyperlink ref="B12" r:id="rId7"/>
-    <hyperlink ref="B16" r:id="rId8"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B6" r:id="rId10"/>
-    <hyperlink ref="B7" r:id="rId11"/>
-    <hyperlink ref="B8" r:id="rId12"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{9D1BE87D-A7DD-4F4F-BF64-3F87FCFECE9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added vap program to spreadsheet source document
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmcnaughton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3143BEF-31D9-44F0-96D1-B882049AF414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -127,12 +126,18 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/respond-lawsuit</t>
+  </si>
+  <si>
+    <t>Voluntary acknowledgment of paternity - VAP</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/voluntary-acknowledgment-parentage-vap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,20 +493,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.44140625" customWidth="1"/>
+    <col min="1" max="1" width="44.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -517,7 +522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -525,7 +530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -533,7 +538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -541,7 +546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -549,7 +554,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -557,7 +562,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -565,7 +570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -573,7 +578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -581,7 +586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -589,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -597,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -605,7 +610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -613,7 +618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -621,7 +626,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -629,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -637,24 +642,33 @@
         <v>19</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
+  <sortState ref="A2:B11">
     <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{9D1BE87D-A7DD-4F4F-BF64-3F87FCFECE9D}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B16" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B17" r:id="rId8"/>
+    <hyperlink ref="B14" r:id="rId9"/>
+    <hyperlink ref="B6" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="B8" r:id="rId12"/>
+    <hyperlink ref="B15" r:id="rId13"/>
+    <hyperlink ref="B18" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Interp Request And Motion To Xlsx Removed Feedback Recommend Scale
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmcnaughton\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FCBD38-9834-485A-B57A-60DA77FF4E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4270"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>name</t>
   </si>
@@ -132,12 +133,24 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/voluntary-acknowledgment-parentage-vap</t>
+  </si>
+  <si>
+    <t>Interpreter request</t>
+  </si>
+  <si>
+    <t>Motion</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/interpreter-request</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/motion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,20 +506,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.453125" customWidth="1"/>
+    <col min="1" max="1" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -522,7 +535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -530,7 +543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -538,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -546,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -554,7 +567,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -562,7 +575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -570,7 +583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -578,7 +591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -586,7 +599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -594,7 +607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -602,73 +615,91 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
     <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B16" r:id="rId6"/>
-    <hyperlink ref="B12" r:id="rId7"/>
-    <hyperlink ref="B17" r:id="rId8"/>
-    <hyperlink ref="B14" r:id="rId9"/>
-    <hyperlink ref="B6" r:id="rId10"/>
-    <hyperlink ref="B7" r:id="rId11"/>
-    <hyperlink ref="B8" r:id="rId12"/>
-    <hyperlink ref="B15" r:id="rId13"/>
-    <hyperlink ref="B18" r:id="rId14"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B20" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B13" r:id="rId15" xr:uid="{FD63B7DB-6A26-4B08-9B48-4F88525F0C73}"/>
+    <hyperlink ref="B15" r:id="rId16" xr:uid="{1BA53872-B2C7-49C3-82A5-F6B1A4E949D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added esignature question, added proof of delivery to easy forms spreadsheet list
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmcnaughton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479845A8-D48C-42D6-AD7E-E9FBE87E1D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5736"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -181,12 +180,18 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/personnel-file-request</t>
+  </si>
+  <si>
+    <t>Proof of delivery</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/proof-delivery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,11 +547,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,78 +722,86 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
+  <sortState ref="A2:B11">
     <sortCondition ref="A2:A11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B23" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B22" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B13" r:id="rId15" xr:uid="{FD63B7DB-6A26-4B08-9B48-4F88525F0C73}"/>
-    <hyperlink ref="B15" r:id="rId16" xr:uid="{1BA53872-B2C7-49C3-82A5-F6B1A4E949D3}"/>
-    <hyperlink ref="B25" r:id="rId17" xr:uid="{9AFA5E71-C374-4881-8D7C-FE6D9806E46B}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{6E4CE347-2D8B-4AF3-9E22-C0F2F94436B2}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{A3205C7C-0D49-4456-8680-9348D85DA68D}"/>
-    <hyperlink ref="B18" r:id="rId20" xr:uid="{D78A8A22-0EAD-4FB4-95CD-1ADA52281F07}"/>
-    <hyperlink ref="B17" r:id="rId21" xr:uid="{F341446E-D160-4D17-A59F-EF839FEA6611}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B24" r:id="rId6"/>
+    <hyperlink ref="B12" r:id="rId7"/>
+    <hyperlink ref="B25" r:id="rId8"/>
+    <hyperlink ref="B22" r:id="rId9"/>
+    <hyperlink ref="B6" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="B8" r:id="rId12"/>
+    <hyperlink ref="B23" r:id="rId13"/>
+    <hyperlink ref="B27" r:id="rId14"/>
+    <hyperlink ref="B13" r:id="rId15"/>
+    <hyperlink ref="B15" r:id="rId16"/>
+    <hyperlink ref="B26" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B18" r:id="rId20"/>
+    <hyperlink ref="B17" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added CanEx program to spreadsheet, language edit
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B13B69-0FEC-4F6E-A76B-5A0556B6A070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952C1FEC-3F0B-4B21-9B4F-2768475AC7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31500" yWindow="-2115" windowWidth="29670" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/name-change-adult</t>
+  </si>
+  <si>
+    <t>Cannabis expungement</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/cannabis-expungement</t>
   </si>
 </sst>
 </file>
@@ -265,9 +271,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +311,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +417,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,232 +613,241 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B26" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B27" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B24" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B25" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B29" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B13" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B15" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B28" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B20" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B19" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B17" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B16" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B27" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B28" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B30" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B20" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B18" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B17" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Extend Time of Eviction to list of easy forms
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivianM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952C1FEC-3F0B-4B21-9B4F-2768475AC7D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5CF383-1C94-40E9-A464-58C951A7A211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/cannabis-expungement</t>
+  </si>
+  <si>
+    <t>Extend time of eviction</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/extend-time-eviction</t>
   </si>
 </sst>
 </file>
@@ -567,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,184 +675,192 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B12">
-    <sortCondition ref="A2:A12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
+    <sortCondition ref="A2:A13"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B27" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B28" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B28" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B29" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B30" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B20" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B18" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B17" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B27" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B31" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B30" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B23" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B21" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B19" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B18" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added crim court fee waiver to easy form xlsx source
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C4E3B2-554B-44A3-8694-DB34AC6EC6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80776F88-3A30-4971-B52F-0773CA6962C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>name</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/security-deposit-complaint</t>
+  </si>
+  <si>
+    <t>Criminal Court fee waiver</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/criminal-court-fee-waiver</t>
   </si>
 </sst>
 </file>
@@ -615,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,295 +683,304 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
-    <sortCondition ref="A2:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
+    <sortCondition ref="A2:A15"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B33" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B36" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B29" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B38" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B37" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B25" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B21" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B19" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B34" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B31" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B38" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B22" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B20" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
-    <hyperlink ref="B10" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B34" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B28" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B31" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B35" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B32" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B11" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
+    <hyperlink ref="B35" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B32" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B36" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B33" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added fin affidavit to easy forms xlsx
</commit_message>
<xml_diff>
--- a/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
+++ b/docassemble/ILAO/data/sources/ilao_docassemble_easy_forms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnewsted\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80776F88-3A30-4971-B52F-0773CA6962C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AEE42B-87F1-4971-ADF0-DA16C59E9A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="264" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>name</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>https://www.illinoislegalaid.org/legal-information/criminal-court-fee-waiver</t>
+  </si>
+  <si>
+    <t>Financial affidavit</t>
+  </si>
+  <si>
+    <t>https://www.illinoislegalaid.org/legal-information/financial-affidavit</t>
   </si>
 </sst>
 </file>
@@ -621,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,193 +761,201 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -955,32 +969,33 @@
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B34" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B16" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B35" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B38" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B31" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B31" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B38" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B26" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B22" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
-    <hyperlink ref="B20" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
+    <hyperlink ref="B32" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B40" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B26" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{E91D49D0-8A8A-49A5-B571-1E3A551885E4}"/>
+    <hyperlink ref="B21" r:id="rId23" xr:uid="{5EB32812-DDAD-43E1-BEC1-0E8706BB78F8}"/>
     <hyperlink ref="B5" r:id="rId24" xr:uid="{A23C6535-E02D-4241-B7AA-C698CCDB6D31}"/>
     <hyperlink ref="B11" r:id="rId25" xr:uid="{5B0358E0-6FC3-4AF8-8E25-62EBF7059C1A}"/>
-    <hyperlink ref="B35" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
-    <hyperlink ref="B29" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
-    <hyperlink ref="B32" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
-    <hyperlink ref="B36" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
-    <hyperlink ref="B33" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
+    <hyperlink ref="B36" r:id="rId26" xr:uid="{1BD2E9FF-F69E-4E59-ACA9-BD41D2D4AE94}"/>
+    <hyperlink ref="B30" r:id="rId27" xr:uid="{620FD2E8-C9D1-4C14-8ED5-17B01AA5DA33}"/>
+    <hyperlink ref="B33" r:id="rId28" xr:uid="{226D490B-4537-4CB5-95DA-F750E9A0919D}"/>
+    <hyperlink ref="B37" r:id="rId29" xr:uid="{285D1364-5954-4A82-B493-EE664C0786D1}"/>
+    <hyperlink ref="B34" r:id="rId30" xr:uid="{BD0F8AFC-EDD1-4D31-AD59-8FAD5E6F7758}"/>
     <hyperlink ref="B7" r:id="rId31" xr:uid="{4EAFCFFB-67EF-4EA4-9306-448CF1D5D183}"/>
+    <hyperlink ref="B16" r:id="rId32" xr:uid="{B1E55B86-EC01-47AD-AA8B-FA1792695821}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>